<commit_message>
data: finalised data models
</commit_message>
<xml_diff>
--- a/files/imdhub-ids.xlsx
+++ b/files/imdhub-ids.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
   <si>
     <t>tableName</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>http://schema.org/Date</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/prov#Person</t>
   </si>
 </sst>
 </file>
@@ -818,7 +821,7 @@
         <v>52</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M11" t="s">
         <v>38</v>
@@ -834,7 +837,7 @@
     <hyperlink ref="L8" r:id="rId6"/>
     <hyperlink ref="L9" r:id="rId7"/>
     <hyperlink ref="L10" r:id="rId8"/>
-    <hyperlink ref="L11" r:id="rId9"/>
+    <hyperlink ref="L11" r:id="rId9" location="Person"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>